<commit_message>
word document is fixed
</commit_message>
<xml_diff>
--- a/results/Models Comparison.xlsx
+++ b/results/Models Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Skin Permeation\Skin-Permeation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B99E73-214B-4314-82FA-042FBB34E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFF45B5-968B-4C4A-B3CB-DC4AE8EADB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,17 +178,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -204,6 +193,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -217,46 +217,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,13 +535,13 @@
   <dimension ref="C5:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -565,7 +559,7 @@
       <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -573,162 +567,162 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="9">
         <v>15.85159</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1.105507</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.56046399999999996</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>3.9814050000000001</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>-12.894212</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>0.29277700000000001</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>0.38738299999999998</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>0.178346</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>0.54108900000000004</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="4">
         <v>0.74337500000000001</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="11">
         <v>0.25854700000000003</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="5">
         <v>0.35332599999999997</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="5">
         <v>0.16334599999999999</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="5">
         <v>0.50847600000000004</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="5">
         <v>0.77337800000000001</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>0.29000900000000002</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>0.387768</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <v>0.17983199999999999</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>0.53852500000000003</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>0.74580199999999996</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="10">
         <v>0.27591199999999999</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>0.37426799999999999</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="4">
         <v>0.17597099999999999</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <v>0.52527299999999999</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>0.758158</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>0.28640500000000002</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>0.38220599999999999</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="4">
         <v>0.178144</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>0.53516799999999998</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>0.74896099999999999</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="10">
         <v>0.48276746834745998</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>0.48291176151661602</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="4">
         <v>0.239405430413207</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>0.69481470072779805</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="4">
         <v>0.57684535396968695</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="10">
         <v>0.54985702755971</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="4">
         <v>0.65628934303919395</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="4">
         <v>0.33912662155203899</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <v>0.74152345044489998</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>6.88314618339258E-2</v>
       </c>
     </row>

</xml_diff>